<commit_message>
Updated files within automation-testing folder
</commit_message>
<xml_diff>
--- a/doctor_names.xlsx
+++ b/doctor_names.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A299"/>
+  <dimension ref="A1:A301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,735 +438,735 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dr. Bikash Rijal</t>
+          <t>Dr. Bharat Pokhrel</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dr. Sudin Kayastha</t>
+          <t>Dr. Ashish Satyal</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Hamro Patro I</t>
+          <t>Dr. Bikash Rijal</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Hamro health</t>
+          <t>Dr. Rika Rijal</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Hamro Patro</t>
+          <t>Dr. Ubaid Ansari</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Dr. Prabhakar Manu</t>
+          <t>Dr. Imran Ansari</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Dr. Samjhana Phuyal</t>
+          <t>Dr. Yujal Man Singh</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Dr. Alok Chandra Thakur</t>
+          <t>Kapil Sharma</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Dr. Shiva Raj Paneru</t>
+          <t>Dr. Abhinav Pradhan</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Dr. Prince Rauniyar</t>
+          <t>Dr. Dibya Sharma</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Dr. Amrit Rijal</t>
+          <t>Dr. Saraswati Bhattarai</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Dr. Pradhumna Kumar Yadav</t>
+          <t>Dr. Ramesh Prasad Aacharya</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Dr. Rajiv Dhakal</t>
+          <t>Hamro Patro I</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Dr. Sabin Adhikari</t>
+          <t>Dr. Sudeep Kr Thakur</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Dr. Dilip Prasad Sah</t>
+          <t>Dr. Poonam Rawal</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Dr. Bhuwan Thapa</t>
+          <t>Hamro health</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Dr. Ashish Satyal</t>
+          <t>Hamro Patro</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Dr. Kushal Shrestha</t>
+          <t>Dr. Prabhakar Manu</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Dr. Pratistha Ghimire</t>
+          <t>Dr. Alok Chandra Thakur</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Dr. Hari Sharan Aryal</t>
+          <t>Dr. Shiva Raj Paneru</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Dr. Sabin Shrestha</t>
+          <t>Dr. Sudip Yadav</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Dr. Saru Shrestha</t>
+          <t>Dr. Akash Rauniyar</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Dr. Sudeep Kr Thakur</t>
+          <t>Dr. Devraj Kshetri</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Dr. Kajal Mehta</t>
+          <t>Dr. Sudhansu Pradhan</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Dr. Sailesh Twanabasu</t>
+          <t>Dr. Rajeev Bhandari</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Dr. Saroj Prasad Ojha</t>
+          <t>Dr. Rachana Koirala</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Dr. Parsuram Sah</t>
+          <t>Dr. Reet Poudel</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Dr. Rasmita Shrestha</t>
+          <t>Dr. Janak Das Kathabaniya</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Dr. Pradip Bhandari</t>
+          <t>Dr. Milan Sedhai</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Dr. Suresh Raj Sharma</t>
+          <t>Dr. Shriya Bastakoti</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Dr. Saroj Prasad Deo</t>
+          <t>Dr. Saru Shrestha</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Dr. Sumedh Mishra</t>
+          <t>Dr. Rajan Govinda Mulmi</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Dr. Manish Basnet</t>
+          <t>Dr. Bhuwan Thapa</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Dr. Poonam Rawal</t>
+          <t>Dr. Shamini Chaudhary</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Dr. Swaraj Udas</t>
+          <t>Dr. Praveen Mandal</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Dr. Sima Ghimire</t>
+          <t>Dr. Roshan Khatiwada</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Dr. Hari Prasad Gyawali</t>
+          <t>Dr. Jagat Jeevan Ghimire</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Dr. Binaya Kamat</t>
+          <t>Dr. Shubhechchhya Amatya</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Dr. Devraj Kshetri</t>
+          <t>Dr. Rupesh Kumar Mahato</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Dr. Sudarshan Kandel</t>
+          <t>Dr. Saroj Prasad Ojha</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Dr. Dhiraj Bishankha</t>
+          <t>Dr. Jamal Ashraf</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Dr. Kavindra Thapa</t>
+          <t>Dr. Isha Poudel Koirala</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Dr. Nabin Simkhada</t>
+          <t>Dr. Nimi Yadav</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Dr. Sudeep Adhikari</t>
+          <t>Dr. Krishma Bhandary</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Dr. Shubhechchhya Amatya</t>
+          <t>Dr. Om Prakash Patel</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Dr. Manish Shrestha</t>
+          <t>Dr. Archana Yadav</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Dr. Anuj Shrestha</t>
+          <t>Dr. Sabin Shrestha</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Dr. Sandesh Lamsal</t>
+          <t>Dr. Anjana Sapkota</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Dr. Raj Kumar BK</t>
+          <t>Dr. Kushal Shrestha</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Dr. Rajeev Chaudhary</t>
+          <t>Dr. Mitesh Yadav</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Dr. Bharat Pokhrel</t>
+          <t>Dr. Gopal K. Yadav</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Dr. Shriya Bastakoti</t>
+          <t>Dr. Rajan Sharma Kandel</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Dr. Shivendra kumar jha</t>
+          <t>Dr. Mukesh Singh Dhami</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Dr. Sanjay Kumar Yadav</t>
+          <t>Dr. Alok Thaiba</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Dt. Madan Pandey</t>
+          <t>Dr. Nirman Neopane</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Dr. Roshan Khatiwada</t>
+          <t>Dr. Lokeshwor Maharjan</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Dr. Manish Singh</t>
+          <t>Dr. Bikash Shrestha</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Dr. Anjani Kumar Yadav</t>
+          <t>Dr. Bharat khadka</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Dr. Dibya Sharma</t>
+          <t>Dr. Binaya Kamat</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Dr. Aastha Khadka</t>
+          <t>Dr. Shivendra kumar jha</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Dr. Nimi Yadav</t>
+          <t>Dr. Sumedh Mishra</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Dr. Alok Thaiba</t>
+          <t>Dr. Romin Shrestha</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Dr. Subhash Thakur</t>
+          <t>Dr. Bijay Mehta</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Dr. Sumit Prajapati</t>
+          <t>Dr. Swaraj Udas</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Dr. Mohammad Sheraj Husain</t>
+          <t>Dr. Jiwan Paudel</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Dt. Kiran Tiwari</t>
+          <t>Dr. Kajal Mehta</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Dr. Sudip Yadav</t>
+          <t>Dr. Dilip Kunwar</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Dr. Sahadeb Prasad Dhungana</t>
+          <t>Dr. Prakreeti Bhandari</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Dr. Rajeev Bhandari</t>
+          <t>Dr. Suresh Raj Sharma</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Dr. Binaya Raj Ghimire</t>
+          <t>Dr. Sahadeb Prasad Dhungana</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Dr. Mukesh Singh Dhami</t>
+          <t>Dr. Hari Prasad Gyawali</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Dr. Kabita Neupane</t>
+          <t>Dr. Manish Basnet</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Dr. Naresh Bhandari</t>
+          <t>Dr. Sudeep Adhikari</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Dr. Praveen Mandal</t>
+          <t>Dr. Suman Raja Shrestha</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Dr. Manish Acharya</t>
+          <t>Dr. Bidhya Thapaliya</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Dr. Saraswati Bhattarai</t>
+          <t>Dr. Astha Regmi</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Dr. Isha Poudel Koirala</t>
+          <t>Dr. Bimalesh Kumar Gupta</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Dr. Pankaj Pratap Deo</t>
+          <t>Dr. Kavindra Thapa</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Dr. Rachana Koirala</t>
+          <t>Dr. Sima Ghimire</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Dr. Abhishek Chaurasiya</t>
+          <t>Dr. Priyanka Shah</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Dr. Nisha Adhikari</t>
+          <t>Dr. Bal Krishna Shah</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Dr. Pratistha Ghimire</t>
+          <t>Dr. Mani Prasad Gautam</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Dr. Kamal Prasad Thani</t>
+          <t>Dr. Hari Sharan Aryal</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Dr. Bidhan Koirala</t>
+          <t>Dr. Chandra Shekhar Yadav</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Dr. Archana Joshi</t>
+          <t>Dr. Parsuram Sah</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Dr. Aayush Shrestha</t>
+          <t>Dr. Mohammad Sheraj Husain</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Dr. Jitendra Adhikari</t>
+          <t>Dt. Kiran Tiwari</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Kapil Sharma</t>
+          <t>Dr. Shijan Raj Shrestha</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Dr. Suman Raja Shrestha</t>
+          <t>Dr. Pradhumna Kumar Yadav</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Dr. Lakpa Dolma Lama</t>
+          <t>Dr. Shristy Khadka</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Dr. Mani Prasad Gautam</t>
+          <t>Dr. Bidhan Koirala</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Dr. Bharat khadka</t>
+          <t>Dr. Rasmita Shrestha</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Dr. Gopal K. Yadav</t>
+          <t>Dt. Madan Pandey</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Dr. Adarsh Gurung</t>
+          <t>Dr. Anjani Kumar Yadav</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Dr. Sabita Singh</t>
+          <t>Dr. Lakpa Dolma Lama</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Dr. Romin Shrestha</t>
+          <t>Dr. Santosh Shrestha</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Dr. Abhinav Pradhan</t>
+          <t>Dr. Sabita Singh</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Dr. Bijay Mehta</t>
+          <t>Dr. Aashish Yadav</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Dr. Jagat Jeevan Ghimire</t>
+          <t>Dr. Rajiv Dhakal</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Dr. Om Prakash Patel</t>
+          <t>Dr. Sabin Paudel</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Dr. Selisha Joshi</t>
+          <t>Dr. Sanjay Kumar Yadav</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Dr. Janak Das Kathabaniya</t>
+          <t>Dr. Samjhana Phuyal</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Dr. Astha Regmi</t>
+          <t>Dr. Abhishek Chaurasiya</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Dr. Sudhansu Pradhan</t>
+          <t>Dr. Manish Acharya</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Dr. Shiva Chaudhary</t>
+          <t>Dr. Saroj Prasad Deo</t>
         </is>
       </c>
     </row>
@@ -1180,98 +1180,98 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Dr. Pradesh Ghimire</t>
+          <t>Dr. Gyanendra Chaudhary</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Dr. Nirman Neopane</t>
+          <t>Dr. Pradip Bhandari</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Dr. Sabin Paudel</t>
+          <t>Dr. Selisha Joshi</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Dr. Gyanendra Chaudhary</t>
+          <t>Dr. Aastha Khadka</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Dr. Priyanka Shah</t>
+          <t>Dr. Khagendra Kafle</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Hemnath Acharya</t>
+          <t>Dr. Subash Mehta</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Dr. Anjana Sapkota</t>
+          <t>Dr. Sudin Kayastha</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Dr. Bidhya Thapaliya</t>
+          <t>Dr. Sailesh Twanabasu</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Dr. Rajan Sharma Kandel</t>
+          <t>Dr. Sabin Adhikari</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Dr. Archana Yadav</t>
+          <t>Dr. Anuj Shrestha</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Dr. Rupesh Kumar Mahato</t>
+          <t>Dr. Rajeev Chaudhary</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Dr. Imran Ansari</t>
+          <t>Dr. Arjun Shrestha</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Dr. Khagendra Kafle</t>
+          <t>Dr. Pratistha Ghimire</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Dr. Jamal Ashraf</t>
+          <t>Dr. Pradesh Ghimire</t>
         </is>
       </c>
     </row>
@@ -1285,224 +1285,224 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Dr. Rika Rijal</t>
+          <t>Dr. Sumit Prajapati</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Dr. Subash Mehta</t>
+          <t>Dr. Dilip Prasad Sah</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Dr. Shamini Chaudhary</t>
+          <t>Dr. Naresh Bhandari</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Dr. Gopesh Kumar Thakur</t>
+          <t>Dr. Pankaj Pratap Deo</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Dr. Arjun Shrestha</t>
+          <t>Dr. Nabin Simkhada</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Dr. Santosh Shrestha</t>
+          <t>Dr. Sandesh Lamsal</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Dr. Milan Sedhai</t>
+          <t>Dr. Anoop Krishna Gupta</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Dr. Chandra Shekhar Yadav</t>
+          <t>Dr. Subhash Thakur</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Dr. Bikash Shrestha</t>
+          <t>Dr. Dhiraj Bishankha</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Dr. Jiwan Paudel</t>
+          <t>Dr. Raj Kumar BK</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Dr. Anoop Krishna Gupta</t>
+          <t>Dr. Kamal Prasad Thani</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Dr. Ashutosh Kumar Badal</t>
+          <t>Dr. Shiva Chaudhary</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Dr. Bimalesh Kumar Gupta</t>
+          <t>Dr. Prasanna Karki</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Dr. Krishma Bhandary</t>
+          <t>Dr. Aayush Shrestha</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Dr. Prakreeti Bhandari</t>
+          <t>Dr Basant Kumar Yadav</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Dr. Mitesh Yadav</t>
+          <t>Dr. Kabita Neupane</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Dr. Shristy Khadka</t>
+          <t>Dr. Gopesh Kumar Thakur</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Dr. Shijan Raj Shrestha</t>
+          <t>Hemnath Acharya</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Dr. Yujal Man Singh</t>
+          <t>Dr. Manish Shrestha</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Dr. Dilip Kunwar</t>
+          <t>Dr. Binaya Raj Ghimire</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Dr. Reet Poudel</t>
+          <t>Dr. Archana Joshi</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Dr. Bal Krishna Shah</t>
+          <t>Dr. Jitendra Adhikari</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Dr. Aashish Yadav</t>
+          <t>Dr. Sudarshan Kandel</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Dr. Lokeshwor Maharjan</t>
+          <t>Dr. Amrit Rijal</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Dr. Prasanna Karki</t>
+          <t>Dr. Pratistha Ghimire</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Dr. Akash Rauniyar</t>
+          <t>Dr. Manish Singh</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Dr. Rajan Govinda Mulmi</t>
+          <t>Dr. Adarsh Gurung</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Dr Basant Kumar Yadav</t>
+          <t>Dr. Nisha Adhikari</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Dr. Mukti Ghimire</t>
+          <t>Dr. Shambhu Dutta Joshi</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Dr. Neeta Timilsina</t>
+          <t>Dr. Rishi Ram Adhikari</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Dr. Shambhu Dutta Joshi</t>
+          <t>Dr. Mukti Ghimire</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Dr. Vikash Paudel</t>
+          <t>Dr. Sonai Chaudhari Giri</t>
         </is>
       </c>
     </row>
@@ -1516,49 +1516,49 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Dr. Deebya Raj Mishra</t>
+          <t>Prof. Dr. Laxman Adhikari</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Dr. Amod Shrestha</t>
+          <t>Dr. Yogendra Mani Basnet</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Dr. Sonai Chaudhari Giri</t>
+          <t>Dr. Amod Shrestha</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Dr. Smriti Mathema</t>
+          <t>Dr. Nirmal Karki</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Dr. Arnab Panta</t>
+          <t>Dr. Birendra Mandal</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Dt. Sukriti Ghimire</t>
+          <t>Dr. Deebya Raj Mishra</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Dr. Birendra Mandal</t>
+          <t>Dt. Sukriti Ghimire</t>
         </is>
       </c>
     </row>
@@ -1600,889 +1600,889 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Dr. Shreesiya Pokharel</t>
+          <t>Dr. Pradeep Bastola</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Dr. Surakshya Baral</t>
+          <t>Dr. Dilesh Pradhan</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Dr. Amuda Regmi</t>
+          <t>Dr. Amin Tuitui</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Dr. Priyanka Giri</t>
+          <t>Dr. Ramesh Sharma</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Dr. Saroj Kumar Suwal</t>
+          <t>Dr. Ashwin Thakali</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Dr. Swarnima Rijal</t>
+          <t>Dr. Shankar Kafle</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Dr. Arun Kumar Singh</t>
+          <t>Dr. Manoj Dhakal</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Dr. Bikash Anand</t>
+          <t>Dr. Shivani Shrestha</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Dr. Suju Bhattrai</t>
+          <t>Dr. Shriya Shrestha</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Dr. Zahir Ansari</t>
+          <t>Dr. Anil Kumar Shrestha</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Dr. Krishna Chandra Mandal</t>
+          <t>Dr. Shishir Pokhrel</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Dr. Pradip Rimal</t>
+          <t>Dr. Shiv Raj Shah</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Dr. Sweta Singh</t>
+          <t>Dr. Jagadish Thapa</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Dr. Shiv Raj Shah</t>
+          <t>Dr. Susan Thapa</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Dr. Mukul Upadhyay Nepal</t>
+          <t>Dr. Priya Bhusal</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Dr. Tilak Bhurtel</t>
+          <t>Dr. Krishna Chandra Mandal</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Dr. Pawan Rauniyar</t>
+          <t>Dr. Deepak Regmi</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Dr. Sunita Karki</t>
+          <t>Dr. Dinuja Khadka</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Dr. Thanesh Neupane</t>
+          <t>Dr. Jeetendra Mandal</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Dr. Gaurav Rajbhandari</t>
+          <t>Dr. Manbodh Kumar Sah</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Dr. Shiva Aryal</t>
+          <t>Dr. Swarnima Rijal</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Dr. Santosh Kumar Thakur</t>
+          <t>Dr. Shubham Sharma</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Dr. Rishi Ram Adhikari</t>
+          <t>Dr. Anil Bhattarai</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Dr. Manbodh Kumar Sah</t>
+          <t>Dr. Mukul Upadhyay Nepal</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Dr. Dhruba Shrestha</t>
+          <t>Dr. Rashila Lamichhane</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Dr. Shriya Shrestha</t>
+          <t>Dr. Nabin Hamal</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Dr. Pragya Singh</t>
+          <t>Dr. Dinesh Kumar B.K</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Dr. Jagadish Thapa</t>
+          <t>Dr. Hari Prasad Baral</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Dr. Animesh Vaidya</t>
+          <t>Dr. Saroj Kumar Suwal</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Dr. Rajesh Lamichhane</t>
+          <t>Dr. Buddhi Prasad Paudel</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Dr. Parash Poudel</t>
+          <t>Dr. Suju Bhattrai</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Dr. Pritee Trivedee</t>
+          <t>Dr. Nitesh Kumar Roy</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Dr. Jyoti Agrawal</t>
+          <t>Dr. Mala Shrestha</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Dr. Manoj Dhakal</t>
+          <t>Dr. Chandan Banerjee</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Dr. Suyash Timalsina</t>
+          <t>Dr. Niraj Kumar Singh</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Dr. Sunita Lamsal</t>
+          <t>Dr. Adarsha Khanal</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Dr. Ganesh Agrawal</t>
+          <t>Dr. Subigya Parajuli</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Dr. Adarsha Khanal</t>
+          <t>Dr. Diwas Bhandari</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Dr. Lokesh Acharya</t>
+          <t>Dr. Anand Mani Upadhyay</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Dr. Ravi Prakash Yadav</t>
+          <t>Dr. Lokesh Acharya</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Dr. Sanju Majakoti</t>
+          <t>Dr. Deepa Khanal</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Dr. Chandan Banerjee</t>
+          <t>Dr. Ujwol Neupane</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Dr. Bikash Bhandari</t>
+          <t>Dr. Sunita Lamsal</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Dr. Deepak Regmi</t>
+          <t>Dr. Anuj Mani Neupane</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Dr. Saroj Singh</t>
+          <t>Dr. Animesh Vaidya</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Dr. Diwas Bhandari</t>
+          <t>Dr. Suman Prasad Adhikari</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Dr. Yogendra Mani Basnet</t>
+          <t>Dr. Shiva Aryal</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Dr. Susan Thapa</t>
+          <t>Dr. Mohir Pokharel</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Dr. Sagar Koirala</t>
+          <t>Dr. Shankar Thapa</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Dr. Shankar Thapa</t>
+          <t>Dr. Pawan Rauniyar</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Dr. Pradeep Bastola</t>
+          <t>Dr. Jyoti Agrawal</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Dr. Prem Tamang</t>
+          <t>Dr. Arnab Panta</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Dr. Shishir Pokhrel</t>
+          <t>Dr. Meen Raj Pathak</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Dr. Himal Khanal</t>
+          <t>Dr. Sachit Devkota</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Dr. Sadikchha Chapagain</t>
+          <t>Hamro Patro Support</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Dr. Gaurav Nepal</t>
+          <t>Dr. Parash Poudel</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Dr. Jeetendra Mandal</t>
+          <t>Dr. Zahir Ansari</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Dr. Dilesh Pradhan</t>
+          <t>Dr. Priyanka Giri</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Dr. Madhav Panthi</t>
+          <t>Dr. Mohan Raj Sharma</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Dr. Sachit Devkota</t>
+          <t>Dr. Gaurav Rajbhandari</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Dr. Ujwol Neupane</t>
+          <t>Dr. Anju Khapung</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Dr. Pratik Bhattarai</t>
+          <t>Dr. Dhruba Shrestha</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Dr. Jitendra Kumar Sah</t>
+          <t>Dr. Shreesiya Pokharel</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Dr. Richa Sah</t>
+          <t>Dr. Appu Jha Avinash</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>Dr. Prami Nakarmi</t>
+          <t>Dr. Nipun Shrestha</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Dr. Anuj Mani Neupane</t>
+          <t>Dr. Ganesh Agrawal</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Dr. Ashwin Thakali</t>
+          <t>Dr. Santosh Kumar Thakur</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Dr. Rashila Lamichhane</t>
+          <t>Dr. Bikash Bhandari</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Dr. Anand Mani Upadhyay</t>
+          <t>Dr. Arun Kumar Mandal</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Dr. Vinayak Regmi</t>
+          <t>Dr. Richa Sah</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Dr. Santosh Bhusal</t>
+          <t>Dr. Bikash Anand</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Dr. Buddhi Prasad Paudel</t>
+          <t>Dr. Bidur Adhikari</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>Dr. Prabal Pradhan</t>
+          <t>Pt. Bibek Khadka</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Dr. Sujit Shrestha</t>
+          <t>Dr. MD Aklakhur Rahaman</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Dr. Khagendra Kumar Jha</t>
+          <t>Dr. Krishna Prasad Paudel</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Dr. Meen Raj Pathak</t>
+          <t>Dr. Alok Shrestha</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>Dr. Tushar Sah</t>
+          <t>Dr. Tilak Bhurtel</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>Pt. Bibek Khadka</t>
+          <t>Dr. Robert Singh Maharjan</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Dr. Priya Bhusal</t>
+          <t>Dr. Pratikshya Ghimire</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>Dr. Anil Kumar Shrestha</t>
+          <t>Dr. Khagendra Kumar Jha</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>Dr. Nipun Shrestha</t>
+          <t>Dr. Ramesh Ghimire</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>Dr. Anju Khapung</t>
+          <t>Dr. Gaurav Nepal</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Dr. Dinuja Khadka</t>
+          <t>Dr. Sujit Shrestha</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Dr. Biken Shrestha</t>
+          <t>Dr. Vinayak Regmi</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>Dr. Bidur Adhikari</t>
+          <t>Pt. Binaya Kandel</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>Dr. Sangam Giri</t>
+          <t>Dr. Robinjung Bhandari</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>Dr. Chhabilal Nepali</t>
+          <t>Dr. Madhav Panthi</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Dr. Nabin Hamal</t>
+          <t>Dr. Ravi Swar</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>Dr. Nitesh Kumar Roy</t>
+          <t>Dr. Stuti Wagle</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Dr. Deepa Khanal</t>
+          <t>Dr. Ajita Paudel</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Dr. Khusbu Agrawal</t>
+          <t>Dr. Niraj Kumar Sharma</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>Dr. Niraj Kumar Singh</t>
+          <t>Dr. Saroj Singh</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Dr. Rakesh Kumar Shah</t>
+          <t>Dr. Prince Rauniyar</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>Dr. Arun Kumar Mandal</t>
+          <t>Dr. Pragya Singh</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Dr. Mohan Raj Sharma</t>
+          <t>Dr. Pritee Trivedee</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>Dr. Krishna Prasad Paudel</t>
+          <t>Dr. Biken Shrestha</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>Dr. Pratikshya Ghimire</t>
+          <t>Dr. Surakshya Baral</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>Dr. Shivani Shrestha</t>
+          <t>Dr. Aseem Bhattarai</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>Dr. Robert Singh Maharjan</t>
+          <t>Dr. Sadikchha Chapagain</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>Dr. Nirmal Karki</t>
+          <t>Dr. Prami Nakarmi</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>Dr. Ramesh Sharma</t>
+          <t>Dr. Sunita Karki</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>Dr. Hari Prasad Baral</t>
+          <t>Dr. Rajesh Lamichhane</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>Dr. Shubham Sharma</t>
+          <t>Dr. Ravi Prakash Yadav</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>Dr. Stuti Wagle</t>
+          <t>Dr. Eliza Karki</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>Hamro Patro Support</t>
+          <t>Dr. Rakesh Kumar Shah</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>Dr. Subigya Parajuli</t>
+          <t>Dr. Neeta Timilsina</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>Sudikshya Acharya</t>
+          <t>Dr. Sweta Singh</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>Dr. Robinjung Bhandari</t>
+          <t>Dr. Amuda Regmi</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>Dr. Niraj Kumar Sharma</t>
+          <t>Dr. Arun Kumar Singh</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>Dr. Ravi Swar</t>
+          <t>Dr. Pratik Bhattarai</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>Dr. Suman Prasad Adhikari</t>
+          <t>Dr. Manasvi Pradhan</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>Dr. Amit Jha</t>
+          <t>Dr. Khusbu Agrawal</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>Dr. Appu Jha Avinash</t>
+          <t>Dr. Pradip Rimal</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>Dr. Sujan Pandey</t>
+          <t>Dr. Prabal Pradhan</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>Dr. Eliza Karki</t>
+          <t>Dr. Sanju Majakoti</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>Dr. Ramesh Ghimire</t>
+          <t>Dr. Amit Jha</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>Dr. Shankar Kafle</t>
+          <t>Sudikshya Acharya</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>Dr. Anil Bhattarai</t>
+          <t>Dr. Vikash Paudel</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>Dr. Arpana Nagila</t>
+          <t>Dr. Suyash Timalsina</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>Dr. Alok Shrestha</t>
+          <t>Dr. Himal Khanal</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>Dr. Amin Tuitui</t>
+          <t>Dr. Jitendra Kumar Sah</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>Dr. Manasvi Pradhan</t>
+          <t>Dr. Tushar Sah</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>Dr. Ajita Paudel</t>
+          <t>Dr. Sangam Giri</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>Pt. Binaya Kandel</t>
+          <t>Dr. Chhabilal Nepali</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>Dr. Mohir Pokharel</t>
+          <t>Dr. Smriti Mathema</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>Dr. Mala Shrestha</t>
+          <t>Dr. Sujan Pandey</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>Dr. Aseem Bhattarai</t>
+          <t>Dr. Thanesh Neupane</t>
         </is>
       </c>
     </row>
@@ -2496,21 +2496,35 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>Prof. Dr. Laxman Adhikari</t>
+          <t>Dr. Ashutosh Kumar Badal</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>Dr. MD Aklakhur Rahaman</t>
+          <t>Dr. Sagar Koirala</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>Dr. Dinesh Kumar B.K</t>
+          <t>Dr. Santosh Bhusal</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>Dr. Prem Tamang</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>Dr. Arpana Nagila</t>
         </is>
       </c>
     </row>

</xml_diff>